<commit_message>
Output de los archivos 100 y 200
</commit_message>
<xml_diff>
--- a/src/output/cabanaconde/4/cargas_trabajo.xlsx
+++ b/src/output/cabanaconde/4/cargas_trabajo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>N.º</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Cargas de trabajo</t>
   </si>
   <si>
-    <t>Programacion</t>
+    <t>Programación</t>
   </si>
   <si>
     <t>Ejecución</t>
@@ -94,22 +94,34 @@
     <t>m</t>
   </si>
   <si>
-    <t>MR400</t>
-  </si>
-  <si>
-    <t>Seguridad vial</t>
-  </si>
-  <si>
-    <t>MR401</t>
-  </si>
-  <si>
-    <t>Conservación de señales</t>
-  </si>
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
-    <t>Ejec. adelantada</t>
+    <t>MR203</t>
+  </si>
+  <si>
+    <t>Limpieza de badén</t>
+  </si>
+  <si>
+    <t>MR300</t>
+  </si>
+  <si>
+    <t>Control de vegetación</t>
+  </si>
+  <si>
+    <t>MR301</t>
+  </si>
+  <si>
+    <t>Roce y limpieza</t>
+  </si>
+  <si>
+    <t>MR700</t>
+  </si>
+  <si>
+    <t>Actividades complementarias</t>
+  </si>
+  <si>
+    <t>MR701</t>
+  </si>
+  <si>
+    <t>Reparación de muros secos</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B7:I16"/>
+  <dimension ref="B7:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -590,10 +602,10 @@
         <v>1.540444444444444</v>
       </c>
       <c r="G10" s="5">
-        <v>3.6</v>
+        <v>1.54</v>
       </c>
       <c r="H10" s="6">
-        <v>2.34</v>
+        <v>1</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>14</v>
@@ -616,10 +628,10 @@
         <v>153.1483333333333</v>
       </c>
       <c r="G11" s="5">
-        <v>360</v>
+        <v>153.2</v>
       </c>
       <c r="H11" s="6">
-        <v>2.35</v>
+        <v>1</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>14</v>
@@ -642,10 +654,10 @@
         <v>17.01125</v>
       </c>
       <c r="G12" s="5">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H12" s="6">
-        <v>0.53</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>14</v>
@@ -677,47 +689,108 @@
         <v>1515.151818181818</v>
       </c>
       <c r="G14" s="5">
-        <v>1440</v>
+        <v>1515.2</v>
       </c>
       <c r="H14" s="6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="3"/>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="5">
+        <v>42.42454545454546</v>
+      </c>
+      <c r="G15" s="5">
+        <v>42.42</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="4">
-        <v>5</v>
-      </c>
+      <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="3" t="s">
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>10</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3606.515454545454</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3606.52</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="4">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3.866</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3.87</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -731,7 +804,7 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:I16">
+  <conditionalFormatting sqref="B7:I19">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(B7))</formula>
     </cfRule>

</xml_diff>